<commit_message>
Updated to support the latest D365 version
</commit_message>
<xml_diff>
--- a/USDFramework/TC_CreateNewCase/Main.rvl.xlsx
+++ b/USDFramework/TC_CreateNewCase/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="110">
   <si>
     <t>Flow</t>
   </si>
@@ -340,6 +340,9 @@
   </si>
   <si>
     <t>Close</t>
+  </si>
+  <si>
+    <t>20000</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="234">
+  <borders count="235">
     <border>
       <left/>
       <right/>
@@ -601,11 +604,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="234">
+  <cellXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -840,6 +844,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="231" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="232" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="233" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="234" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,7 +854,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H45"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.453125" customWidth="true"/>
@@ -1149,33 +1154,31 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="204"/>
+      <c r="A17" s="234"/>
     </row>
     <row r="18">
-      <c r="A18" s="205" t="s">
-        <v>7</v>
-      </c>
+      <c r="A18" s="204"/>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="F18" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G18" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="206" t="s">
+      <c r="A19" s="205" t="s">
         <v>7</v>
       </c>
       <c r="B19" t="s">
@@ -1185,79 +1188,79 @@
         <v>66</v>
       </c>
       <c r="D19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="206" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s">
         <v>68</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>69</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>25</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="218"/>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
+    <row r="21">
+      <c r="A21" s="218"/>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
         <v>103</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>107</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>86</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>87</v>
-      </c>
-      <c r="G20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="233"/>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" t="s">
-        <v>25</v>
       </c>
       <c r="G21" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="221"/>
+      <c r="A22" s="233"/>
       <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="F22" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="G22" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="210" t="s">
-        <v>7</v>
-      </c>
+      <c r="A23" s="221"/>
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -1265,7 +1268,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
@@ -1278,7 +1281,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="211" t="s">
+      <c r="A24" s="210" t="s">
         <v>7</v>
       </c>
       <c r="B24" t="s">
@@ -1288,119 +1291,119 @@
         <v>74</v>
       </c>
       <c r="D24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="211" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" t="s">
         <v>68</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>69</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F25" t="s">
         <v>25</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="212" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
+    <row r="26">
+      <c r="A26" s="212" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
         <v>76</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>67</v>
       </c>
-      <c r="E25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="213" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="213" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
         <v>77</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>78</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>79</v>
-      </c>
-      <c r="F26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="214" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" t="s">
-        <v>80</v>
       </c>
       <c r="F27" t="s">
         <v>28</v>
       </c>
       <c r="G27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="214" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="215" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
+    <row r="29">
+      <c r="A29" s="215" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
         <v>82</v>
-      </c>
-      <c r="D28" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="216" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
       </c>
       <c r="D29" t="s">
         <v>67</v>
@@ -1416,14 +1419,14 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="217" t="s">
+      <c r="A30" s="216" t="s">
         <v>7</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
         <v>67</v>
@@ -1439,114 +1442,137 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="196"/>
+      <c r="A31" s="217" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="81"/>
-      <c r="B32" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="83" t="s">
+      <c r="A32" s="196"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="81"/>
+      <c r="B33" s="82" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="83" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="84" t="s">
+      <c r="D33" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="E32" s="85" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="87" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="88"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="105"/>
-      <c r="B33" s="106"/>
-      <c r="C33" s="107"/>
-      <c r="D33" s="108"/>
-      <c r="E33" s="109"/>
-      <c r="F33" s="110"/>
-      <c r="G33" s="111"/>
-      <c r="H33" s="112"/>
+      <c r="E33" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="87" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="88"/>
     </row>
     <row r="34">
-      <c r="A34" s="113"/>
-      <c r="B34" s="114"/>
-      <c r="C34" s="115"/>
-      <c r="D34" s="116"/>
-      <c r="E34" s="117"/>
-      <c r="F34" s="118"/>
-      <c r="G34" s="119"/>
-      <c r="H34" s="120"/>
+      <c r="A34" s="105"/>
+      <c r="B34" s="106"/>
+      <c r="C34" s="107"/>
+      <c r="D34" s="108"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="110"/>
+      <c r="G34" s="111"/>
+      <c r="H34" s="112"/>
     </row>
     <row r="35">
-      <c r="A35" s="121"/>
-      <c r="B35" s="122"/>
-      <c r="C35" s="123"/>
-      <c r="D35" s="124"/>
-      <c r="E35" s="125"/>
-      <c r="F35" s="126"/>
-      <c r="G35" s="127"/>
-      <c r="H35" s="128"/>
+      <c r="A35" s="113"/>
+      <c r="B35" s="114"/>
+      <c r="C35" s="115"/>
+      <c r="D35" s="116"/>
+      <c r="E35" s="117"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="119"/>
+      <c r="H35" s="120"/>
     </row>
     <row r="36">
-      <c r="A36" s="129"/>
-      <c r="B36" s="130"/>
-      <c r="C36" s="131"/>
-      <c r="D36" s="132"/>
-      <c r="E36" s="133"/>
-      <c r="F36" s="134"/>
-      <c r="G36" s="135"/>
-      <c r="H36" s="136"/>
+      <c r="A36" s="121"/>
+      <c r="B36" s="122"/>
+      <c r="C36" s="123"/>
+      <c r="D36" s="124"/>
+      <c r="E36" s="125"/>
+      <c r="F36" s="126"/>
+      <c r="G36" s="127"/>
+      <c r="H36" s="128"/>
     </row>
     <row r="37">
-      <c r="A37" s="137"/>
-      <c r="B37" s="138"/>
-      <c r="C37" s="139"/>
-      <c r="D37" s="140"/>
-      <c r="E37" s="141"/>
-      <c r="F37" s="142"/>
-      <c r="G37" s="143"/>
-      <c r="H37" s="144"/>
+      <c r="A37" s="129"/>
+      <c r="B37" s="130"/>
+      <c r="C37" s="131"/>
+      <c r="D37" s="132"/>
+      <c r="E37" s="133"/>
+      <c r="F37" s="134"/>
+      <c r="G37" s="135"/>
+      <c r="H37" s="136"/>
     </row>
     <row r="38">
-      <c r="A38" s="145"/>
-      <c r="B38" s="146"/>
-      <c r="C38" s="147"/>
-      <c r="D38" s="148"/>
-      <c r="E38" s="149"/>
-      <c r="F38" s="150"/>
-      <c r="G38" s="151"/>
-      <c r="H38" s="152"/>
+      <c r="A38" s="137"/>
+      <c r="B38" s="138"/>
+      <c r="C38" s="139"/>
+      <c r="D38" s="140"/>
+      <c r="E38" s="141"/>
+      <c r="F38" s="142"/>
+      <c r="G38" s="143"/>
+      <c r="H38" s="144"/>
     </row>
     <row r="39">
-      <c r="A39" s="153"/>
-      <c r="B39" s="154"/>
-      <c r="C39" s="155"/>
-      <c r="D39" s="156"/>
-      <c r="E39" s="157"/>
-      <c r="F39" s="158"/>
-      <c r="G39" s="159"/>
-      <c r="H39" s="160"/>
+      <c r="A39" s="145"/>
+      <c r="B39" s="146"/>
+      <c r="C39" s="147"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="149"/>
+      <c r="F39" s="150"/>
+      <c r="G39" s="151"/>
+      <c r="H39" s="152"/>
     </row>
     <row r="40">
-      <c r="A40" s="197"/>
+      <c r="A40" s="153"/>
+      <c r="B40" s="154"/>
+      <c r="C40" s="155"/>
+      <c r="D40" s="156"/>
+      <c r="E40" s="157"/>
+      <c r="F40" s="158"/>
+      <c r="G40" s="159"/>
+      <c r="H40" s="160"/>
     </row>
     <row r="41">
-      <c r="A41" s="198"/>
+      <c r="A41" s="197"/>
     </row>
     <row r="42">
-      <c r="A42" s="199"/>
+      <c r="A42" s="198"/>
     </row>
     <row r="43">
-      <c r="A43" s="200"/>
+      <c r="A43" s="199"/>
     </row>
     <row r="44">
-      <c r="A44" s="201"/>
+      <c r="A44" s="200"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="201"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>